<commit_message>
Additional input data updates for 2.1.1
</commit_message>
<xml_diff>
--- a/InputData/dist-heat/EoCtUH/Efficiency of Conversion to Usable Heat.xlsx
+++ b/InputData/dist-heat/EoCtUH/Efficiency of Conversion to Usable Heat.xlsx
@@ -1,27 +1,38 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22624"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipI\InputData\dist-heat\EoCtUH\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeff-nonadmin\CodeRepositories\eps-us\InputData\dist-heat\EoCtUH\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{843E5DCE-5BE1-48F8-B588-2575D3565297}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="45" windowWidth="23955" windowHeight="11310"/>
+    <workbookView xWindow="1125" yWindow="1470" windowWidth="14595" windowHeight="14490" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
     <sheet name="Data" sheetId="2" r:id="rId2"/>
     <sheet name="EoCtUH" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="55">
   <si>
     <t>Source:</t>
   </si>
@@ -80,20 +91,123 @@
     <t>EoCtUH Efficiency of Conversion to Usable Heat</t>
   </si>
   <si>
-    <t>District heat</t>
-  </si>
-  <si>
     <t>Efficiency (dimensionless)</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>coal</t>
+  </si>
+  <si>
+    <t>natural gas</t>
+  </si>
+  <si>
+    <t>biomass</t>
+  </si>
+  <si>
+    <t>petroleum diesel</t>
+  </si>
+  <si>
+    <t>heat</t>
+  </si>
+  <si>
+    <t>crude oil</t>
+  </si>
+  <si>
+    <t>heavy or residual fuel oil</t>
+  </si>
+  <si>
+    <t>LPG propane or butane</t>
+  </si>
+  <si>
+    <t>hydrogen</t>
+  </si>
+  <si>
+    <t>Heat Pump Representation and Electricity</t>
+  </si>
+  <si>
+    <t>for the "electricity" fuel type in this variable.</t>
+  </si>
+  <si>
+    <t>Usable Heat Efficiency</t>
+  </si>
+  <si>
+    <t>Heat Pump Efficiency (Coefficient of Peformance)</t>
+  </si>
+  <si>
+    <t>European Heat Pump Association</t>
+  </si>
+  <si>
+    <t>Large Scale Heat Pumps in Europe: 16 Examples of Realized Projects</t>
+  </si>
+  <si>
+    <t>https://www.ehpa.org/fileadmin/red/03._Media/03.02_Studies_and_reports/Large_heat_pumps_in_Europe_MDN_II_final4_small.pdf</t>
+  </si>
+  <si>
+    <t>Heat Pumps</t>
+  </si>
+  <si>
+    <t>Project number</t>
+  </si>
+  <si>
+    <t>COP</t>
+  </si>
+  <si>
+    <t>Use</t>
+  </si>
+  <si>
+    <t>district heating system</t>
+  </si>
+  <si>
+    <t>paper factory</t>
+  </si>
+  <si>
+    <t>university</t>
+  </si>
+  <si>
+    <t>hospital</t>
+  </si>
+  <si>
+    <t>concrete plant</t>
+  </si>
+  <si>
+    <t>office building (ice storage)</t>
+  </si>
+  <si>
+    <t>office building</t>
+  </si>
+  <si>
+    <t>food processing</t>
+  </si>
+  <si>
+    <t>chipboard factory</t>
+  </si>
+  <si>
+    <t>Avgerage of all district heating system heat pumps</t>
+  </si>
+  <si>
+    <t>Heat generated by a heat pump is still lost in the distribution network, so the overall</t>
+  </si>
+  <si>
+    <t>efficiency of the heat pump systems is the COP multiplied by the efficiency ratio above.</t>
+  </si>
+  <si>
+    <t>Heat pump district heat final delivered efficiency</t>
+  </si>
+  <si>
+    <t>Heat pumps are represented by using an efficiency greater than 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <numFmts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="171" formatCode="0.0"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -125,13 +239,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -150,7 +284,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -159,8 +293,21 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="171" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -256,6 +403,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -291,6 +455,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -466,8 +647,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -485,98 +666,153 @@
       <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" s="2">
         <v>2014</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="3" t="s">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B7" s="3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="4" t="s">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="4"/>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B10" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="16">
+        <v>2018</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B13" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B14" s="8" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>16</v>
       </c>
     </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>31</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B14" r:id="rId1" xr:uid="{5E084D22-3871-4C9B-A603-594DF5DB766D}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="46.42578125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -635,9 +871,231 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="12">
         <f>AVERAGE(A3:G3)</f>
         <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>39</v>
+      </c>
+      <c r="C10" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C11" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>3.1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>3</v>
+      </c>
+      <c r="B13">
+        <v>3.05</v>
+      </c>
+      <c r="C13" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>4</v>
+      </c>
+      <c r="B14">
+        <v>6.7</v>
+      </c>
+      <c r="C14" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15">
+        <v>5.3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6</v>
+      </c>
+      <c r="B16">
+        <v>3.4</v>
+      </c>
+      <c r="C16" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>7</v>
+      </c>
+      <c r="B17">
+        <v>4.8</v>
+      </c>
+      <c r="C17" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>8</v>
+      </c>
+      <c r="B18">
+        <v>6.8</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>9</v>
+      </c>
+      <c r="B19">
+        <v>4.8</v>
+      </c>
+      <c r="C19" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>10</v>
+      </c>
+      <c r="B20">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="C20" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>11</v>
+      </c>
+      <c r="B21" s="13">
+        <v>5</v>
+      </c>
+      <c r="C21" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>12</v>
+      </c>
+      <c r="B22">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>13</v>
+      </c>
+      <c r="B23">
+        <v>3.4</v>
+      </c>
+      <c r="C23" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>14</v>
+      </c>
+      <c r="B24" s="13">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>15</v>
+      </c>
+      <c r="B25">
+        <v>2.6</v>
+      </c>
+      <c r="C25" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>16</v>
+      </c>
+      <c r="B26">
+        <v>4.5</v>
+      </c>
+      <c r="C26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B28" s="14">
+        <f>AVERAGEIFS(B11:B26,C11:C26,"district heating system")</f>
+        <v>3.6642857142857141</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B32" s="15">
+        <f>A6*B28</f>
+        <v>2.5702346938775507</v>
       </c>
     </row>
   </sheetData>
@@ -646,33 +1104,112 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.42578125" customWidth="1"/>
     <col min="2" max="2" width="15.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="45" x14ac:dyDescent="0.25">
-      <c r="B1" s="6" t="s">
-        <v>20</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B2" s="5">
-        <f>Data!A6</f>
+        <f>Data!B32</f>
+        <v>2.5702346938775507</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="5">
+        <f>Data!A$6</f>
+        <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B4" s="5">
+        <f>Data!A$6</f>
+        <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5" s="5">
+        <f>Data!A$6</f>
+        <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" s="5">
+        <f>Data!A$6</f>
+        <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" s="5">
+        <f>Data!A$6</f>
+        <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" s="5">
+        <f>Data!A$6</f>
+        <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>27</v>
+      </c>
+      <c r="B9" s="5">
+        <f>Data!A$6</f>
+        <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" s="5">
+        <f>Data!A$6</f>
+        <v>0.7014285714285714</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="5">
+        <f>Data!A$6</f>
         <v>0.7014285714285714</v>
       </c>
     </row>

</xml_diff>